<commit_message>
AIP-302 AIP-335 Updated the Test Data
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/MaxDFR.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/MaxDFR.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F37BA2-A788-457F-9833-A9F2C89F5C44}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3728DDEB-044D-4866-A3A4-C81BC00AF03C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>DeviceName</t>
   </si>
@@ -49,9 +49,6 @@
     <t>PrefaultTime</t>
   </si>
   <si>
-    <t>2569</t>
-  </si>
-  <si>
     <t>IND_DAU_51</t>
   </si>
   <si>
@@ -79,7 +76,22 @@
     <t>MaxDFR</t>
   </si>
   <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>1200</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
     <t>30000</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
 </sst>
 </file>
@@ -398,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,16 +453,16 @@
         <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -461,30 +473,100 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1">
         <v>409026540</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>409026540</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>409026540</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AIP-305 AIP-348 Test Script for CAM_690
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/MaxDFR.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/MaxDFR.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3728DDEB-044D-4866-A3A4-C81BC00AF03C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEF07FD-06FE-40D9-8B28-20295FDE74DB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
   <si>
     <t>DeviceName</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>1000</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -410,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,6 +573,76 @@
         <v>19</v>
       </c>
     </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
+        <v>409026540</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>409026540</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>